<commit_message>
Update Repeatability_40 sperm batch.xlsx
</commit_message>
<xml_diff>
--- a/Data/Repeatability_40 sperm batch.xlsx
+++ b/Data/Repeatability_40 sperm batch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ds\raw_data_kemp\LAB\Kim\WADERS\Ruff\Sperm Project 2021\Repeatability_40 sperm batch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinbulla/Dropbox/Science/DATA_collection/ruff_sperm/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1634A3A3-8EAC-4033-970E-EAB169D34B3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2C86D7-C3AD-9649-8322-058CEF9CABEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="0" windowWidth="27855" windowHeight="14610" xr2:uid="{66A58A7C-96DC-492F-A980-BCCD1D706852}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{66A58A7C-96DC-492F-A980-BCCD1D706852}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -188,7 +188,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,13 +209,26 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -230,8 +243,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,20 +563,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3411CB36-5014-4FA9-A170-FA6E661E10BF}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -593,7 +608,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -613,17 +628,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>652</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>3</v>
       </c>
       <c r="E3">
@@ -633,7 +648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -653,27 +668,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>605</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>609</v>
       </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -693,7 +708,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -706,14 +721,14 @@
       <c r="D7">
         <v>3</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>855</v>
       </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -733,7 +748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -753,7 +768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -773,17 +788,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>868</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>2</v>
       </c>
       <c r="E11">
@@ -793,7 +808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -806,14 +821,14 @@
       <c r="D12">
         <v>2</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>1395</v>
       </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -826,14 +841,14 @@
       <c r="D13">
         <v>3</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>1785</v>
       </c>
-      <c r="F13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -853,7 +868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -873,7 +888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -886,14 +901,14 @@
       <c r="D16">
         <v>3</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>1745</v>
       </c>
-      <c r="F16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -913,7 +928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -933,7 +948,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -953,7 +968,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -973,7 +988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>

</xml_diff>